<commit_message>
new production version 1.71 add control of output enable of led drivers to fix power on problems when the Battery is connected
git-svn-id: file:///Users/administrator/mobots/svn/electronics/thymio2/trunk@911 56f7f59e-b348-0410-8d88-ca71a75c094d
</commit_message>
<xml_diff>
--- a/output/Bill of Materials-thymio2-main(Production Thymio2).xlsx
+++ b/output/Bill of Materials-thymio2-main(Production Thymio2).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="14625"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22116" windowHeight="10848"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-thymio2-main(" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="204">
   <si>
     <t>Quantity</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>LibRef</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -37,9 +34,6 @@
     <t>Motor connector 89400-0220</t>
   </si>
   <si>
-    <t>Motor</t>
-  </si>
-  <si>
     <t>B1, B2</t>
   </si>
   <si>
@@ -52,9 +46,6 @@
     <t>Battery connector 89400-0220</t>
   </si>
   <si>
-    <t>Battery</t>
-  </si>
-  <si>
     <t>BT1</t>
   </si>
   <si>
@@ -64,10 +55,7 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>100nF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>C1, C3, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C22, C23, C24, C25, C26, C27, C28, C29, C30, C33, C35, C36, C37, C38, C39, C55, C62, C65, C66, C67, C68, C69, C70, C71</t>
+    <t>C1, C3, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C22, C23, C24, C25, C26, C27, C28, C29, C30, C33, C35, C36, C37, C38, C39, C55, C62, C65, C66, C67, C68, C69, C70, C71, C74, C75</t>
   </si>
   <si>
     <t>Capacitor</t>
@@ -79,45 +67,30 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>10uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1, 4.7uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1, 4.7uF[[/\]]0603[[/\]]1, 10uF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>C2, C4, C32, C46, C51, C52, C72, C73</t>
+    <t>C2, C4, C31, C40, C46, C51, C52, C73</t>
   </si>
   <si>
     <t>4.7nF</t>
   </si>
   <si>
-    <t>CAP-NP</t>
-  </si>
-  <si>
     <t>C15, C16, C17, C18, C19, C20, C21</t>
   </si>
   <si>
     <t>4.7uF</t>
   </si>
   <si>
-    <t>4.7uF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>C31, C40, C43, C44, C45, C47, C48, C49, C50</t>
+    <t>C32, C43, C44, C45, C47, C48, C49, C50, C72</t>
   </si>
   <si>
     <t>10uF X5R</t>
   </si>
   <si>
-    <t>10uF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>C34</t>
   </si>
   <si>
     <t>18pF</t>
   </si>
   <si>
-    <t>10pF[[/\]]0603[[/\]]3</t>
-  </si>
-  <si>
     <t>C41, C42</t>
   </si>
   <si>
@@ -133,27 +106,18 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>4.7uF[[/\]]0603[[/\]]1, 1uF[[/\]]0603[[/\]]1, 1uF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>C56, C61, C63</t>
   </si>
   <si>
     <t>1.5nF</t>
   </si>
   <si>
-    <t>10nF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>C57</t>
   </si>
   <si>
     <t>47nF</t>
   </si>
   <si>
-    <t>470nF[[/\]]0603[[/\]]1, 10nF[[/\]]0603[[/\]]1, 470nF[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>C58, C59, C60</t>
   </si>
   <si>
@@ -166,9 +130,6 @@
     <t>19-21SURC/S530-A3/TR8</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>D1, D3, D4, D5</t>
   </si>
   <si>
@@ -181,9 +142,6 @@
     <t>BT5050RGBC-T180</t>
   </si>
   <si>
-    <t>LED RGB SMD 2</t>
-  </si>
-  <si>
     <t>D2, D6, D27, D38</t>
   </si>
   <si>
@@ -202,7 +160,7 @@
     <t>SMD Red led right angle mount 2V@20ma 57mcd</t>
   </si>
   <si>
-    <t>27-21 Everlight</t>
+    <t>27-21 EVERLIGHT</t>
   </si>
   <si>
     <t>27-21/BHC-AN1P2/3C</t>
@@ -235,7 +193,7 @@
     <t>Red led 2V@20ma 57mcd</t>
   </si>
   <si>
-    <t>Led_TH_3mm_20mm</t>
+    <t>LED_TH_3MM_20MM</t>
   </si>
   <si>
     <t>APTD1608CGCK</t>
@@ -262,9 +220,6 @@
     <t>MLP2520S3R3S</t>
   </si>
   <si>
-    <t>IND</t>
-  </si>
-  <si>
     <t>L1, L2, L3, L4</t>
   </si>
   <si>
@@ -289,9 +244,6 @@
     <t>TD4015BPN</t>
   </si>
   <si>
-    <t>Micro1</t>
-  </si>
-  <si>
     <t>MC1</t>
   </si>
   <si>
@@ -304,7 +256,7 @@
     <t>BC817-40</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q15, Q16, Q17, Q18, Q19, Q20, Q21, Q22, Q23, Q24, Q25, Q26, Q27, Q28, Q29, Q30, Q31, Q32, Q33, Q34, Q35, Q36, Q37, Q38, Q39, Q40, Q41, Q42, Q43, Q44, Q45, Q46</t>
+    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q15, Q16, Q17, Q18, Q19, Q20, Q21, Q22, Q23, Q24, Q25, Q26, Q27, Q28, Q29, Q30, Q31, Q32, Q33, Q34, Q35, Q36, Q37, Q38, Q39, Q40, Q41, Q42, Q43, Q44, Q45, Q46, Q47, Q48</t>
   </si>
   <si>
     <t>NPN General-purpose Transistor</t>
@@ -313,10 +265,7 @@
     <t>4.7K</t>
   </si>
   <si>
-    <t>4.7K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>R1, R2, R57, R59, R61, R63, R64, R65, R67, R92, R93, R94, R103, R104, R111, R112, R113, R114, R142, R144, R145, R146</t>
+    <t>R1, R2, R57, R59, R61, R63, R64, R65, R67, R92, R93, R94, R111, R112, R113, R114, R142, R144, R145, R146</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -328,9 +277,6 @@
     <t>33</t>
   </si>
   <si>
-    <t>RES, RES, RES, RES, RES, RES, RES, RES, RES, RES, RES, 68K[[/\]]0603[[/\]]1, RES, RES, RES, 68K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R3, R5, R68, R69, R70, R71, R72, R73, R98, R99, R100, R135, R147, R148, R149, R150</t>
   </si>
   <si>
@@ -340,18 +286,12 @@
     <t>2.7K</t>
   </si>
   <si>
-    <t>RES</t>
-  </si>
-  <si>
     <t>R4, R6</t>
   </si>
   <si>
     <t>22K</t>
   </si>
   <si>
-    <t>RES, RES, RES, RES, RES, RES, RES, 22K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R7, R8, R9, R10, R11, R42, R43, R130</t>
   </si>
   <si>
@@ -361,13 +301,10 @@
     <t>2.2K</t>
   </si>
   <si>
-    <t>RES, RES, RES, RES, RES, 2.2K[[/\]]0603[[/\]]1, 2.2K[[/\]]0603[[/\]]1, 2.2K[[/\]]0603[[/\]]1, 2.2K[[/\]]0603[[/\]]1, 2.2K[[/\]]0603[[/\]]1, RES, RES, 2.2K[[/\]]0603[[/\]]1, 2.2K[[/\]]0603[[/\]]1, 2.2K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>R12, R13, R14, R15, R16, R32, R33, R34, R35, R41, R44, R45, R52, R53, R126</t>
-  </si>
-  <si>
-    <t>120, 120, 120, 120, 120, Resistor, Resistor, Resistor, Resistor, Resistor, 120, 120, Resistor, Resistor, Resistor</t>
+    <t>R12, R13, R14, R15, R16, R32, R33, R34, R35, R41, R44, R45, R52, R53, R103, R104, R126</t>
+  </si>
+  <si>
+    <t>120, 120, 120, 120, 120, Resistor, Resistor, Resistor, Resistor, Resistor, 120, 120, Resistor, Resistor, Resistor, Resistor, Resistor</t>
   </si>
   <si>
     <t>1.5K</t>
@@ -382,18 +319,12 @@
     <t>1K</t>
   </si>
   <si>
-    <t>RES, RES, RES, RES, RES, RES, RES, 1K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R21, R22, R23, R24, R25, R48, R49, R108</t>
   </si>
   <si>
     <t>10K</t>
   </si>
   <si>
-    <t>RES, RES, RES, RES, RES, RES, RES, 10K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]1, 8.2K[[/\]]0603[[/\]]2, 8.2K[[/\]]0603[[/\]]2, 10K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]2</t>
-  </si>
-  <si>
     <t>R27, R28, R29, R30, R31, R50, R51, R101, R102, R109, R110, R117, R118, R128, R129, R136</t>
   </si>
   <si>
@@ -409,9 +340,6 @@
     <t>56</t>
   </si>
   <si>
-    <t>68K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R56, R58, R60, R62, R74, R75, R76, R77, R78, R79, R80, R81, R90, R91</t>
   </si>
   <si>
@@ -424,9 +352,6 @@
     <t>100</t>
   </si>
   <si>
-    <t>RES_ACORT</t>
-  </si>
-  <si>
     <t>R105, R106</t>
   </si>
   <si>
@@ -439,54 +364,36 @@
     <t>180</t>
   </si>
   <si>
-    <t>180R[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R107, R137</t>
   </si>
   <si>
     <t>5.6K</t>
   </si>
   <si>
-    <t>2.2K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R115, R116</t>
   </si>
   <si>
     <t>100K</t>
   </si>
   <si>
-    <t>100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1, 10K[[/\]]0603[[/\]]1, 100K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
-    <t>R119, R120, R121, R122, R123, R124, R138, R139, R141, R143</t>
+    <t>R119, R120, R121, R122, R123, R124, R138, R139, R141, R143, R155, R156, R157, R158, R159</t>
   </si>
   <si>
     <t>680K</t>
   </si>
   <si>
-    <t>470K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R125</t>
   </si>
   <si>
     <t>6.8K</t>
   </si>
   <si>
-    <t>10K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R127</t>
   </si>
   <si>
     <t>820</t>
   </si>
   <si>
-    <t>22K[[/\]]0603[[/\]]1</t>
-  </si>
-  <si>
     <t>R131, R151, R152, R153, R154</t>
   </si>
   <si>
@@ -499,18 +406,12 @@
     <t>270K</t>
   </si>
   <si>
-    <t>270K[[/\]]0603[[/\]]2</t>
-  </si>
-  <si>
     <t>R140</t>
   </si>
   <si>
     <t>NCP15XH103F03RC</t>
   </si>
   <si>
-    <t>Res Thermal</t>
-  </si>
-  <si>
     <t>RT1</t>
   </si>
   <si>
@@ -523,9 +424,6 @@
     <t>MicroSD-Astron 5190008-XA4-R</t>
   </si>
   <si>
-    <t>SD-Card-Micro-ASLTRON 5190008-XA4-R</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -547,7 +445,7 @@
     <t>FSMRA2JH</t>
   </si>
   <si>
-    <t>DMG1013T</t>
+    <t>DMP21DOUT-7</t>
   </si>
   <si>
     <t>T1, T2, T3, T4</t>
@@ -625,9 +523,6 @@
     <t>AP7331-33WG-7</t>
   </si>
   <si>
-    <t>AP7331</t>
-  </si>
-  <si>
     <t>U18, U22, U24, U26</t>
   </si>
   <si>
@@ -649,22 +544,19 @@
     <t>TQFP-PT64_N</t>
   </si>
   <si>
-    <t>IRM-3636T</t>
-  </si>
-  <si>
-    <t>TSOP32236</t>
+    <t>IRM-3638T</t>
   </si>
   <si>
     <t>U20</t>
   </si>
   <si>
-    <t>IR Receiver Module (36 kHz) for Remote Control Systems</t>
+    <t>IR Receiver Module (38 kHz) for Remote Control Systems</t>
   </si>
   <si>
     <t>IR-receiver</t>
   </si>
   <si>
-    <t>MCP73871-2AAI/ML</t>
+    <t>MCP73871-2CAI/ML</t>
   </si>
   <si>
     <t>U21</t>
@@ -685,7 +577,7 @@
     <t>USB/Charger and Over Voltage Detection Device</t>
   </si>
   <si>
-    <t>MLP 1.45x1mm</t>
+    <t>MLP 1.45X1MM</t>
   </si>
   <si>
     <t>LM4819M</t>
@@ -715,28 +607,25 @@
     <t>Alstron R3190005-021-R</t>
   </si>
   <si>
-    <t>USB_MINIAB</t>
-  </si>
-  <si>
     <t>X3</t>
   </si>
   <si>
     <t>USB connector Micro B</t>
   </si>
   <si>
-    <t>Astron 3190005-x21-r</t>
+    <t>ASTRON 3190005-X21-R</t>
   </si>
   <si>
     <t>815-ABLS-8-B2</t>
   </si>
   <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Surface Mount Quartz Crystal 8Mhz</t>
+  </si>
+  <si>
     <t>HC49/4H_SMX</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>Surface Mount Quartz Crystal 8Mhz</t>
   </si>
 </sst>
 </file>
@@ -754,7 +643,7 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1107,21 +996,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1137,1288 +1025,1093 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>48</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="E26" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>46</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>22</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>2</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>8</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>8</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>16</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>14</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>14</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>1</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>5</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>1</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>159</v>
+        <v>84</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>1</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>1</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>4</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>4</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>1</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>2</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>2</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>7</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>5</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>4</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>1</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>1</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>1</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>1</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>1</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>1</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>1</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>1</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>1</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>1</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>1</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>1</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>1</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>1</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>